<commit_message>
end branch: final push
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G531QC\OneDrive\FSJS H8\Phase_3\final project\synapse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC8F54B-E2AB-47A2-B015-78986E12F0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3844C8F9-EF9C-4A61-A54D-F295ACD9D4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9266" yWindow="-18514" windowWidth="17725" windowHeight="17880" xr2:uid="{D2D7A30A-FD97-4444-AF1F-0EF9A96489A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>SERVICE</t>
   </si>
@@ -47,9 +47,6 @@
     <t>DB</t>
   </si>
   <si>
-    <t>Desc</t>
-  </si>
-  <si>
     <t>apiManager</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>analytics</t>
   </si>
   <si>
-    <t>GET /users/:email</t>
-  </si>
-  <si>
     <t>Users, Companies</t>
   </si>
   <si>
@@ -141,6 +135,35 @@
   </si>
   <si>
     <t>new data from miner</t>
+  </si>
+  <si>
+    <t>POST /users</t>
+  </si>
+  <si>
+    <t>token:
+{
+      origin: 'Orchestrator-1'
+    }
+body: {
+  email: str,
+  password: str-hash
+}</t>
+  </si>
+  <si>
+    <t>Req</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>res: {
+  statusCode: 200,
+  data: {
+    email: str,
+    CompanyId: INT,
+    companyName: str
+  }
+}</t>
   </si>
 </sst>
 </file>
@@ -212,9 +235,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -223,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4C204F-1896-4A4F-BA1C-B4F55B5058F3}">
-  <dimension ref="A2:E15"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,12 +592,12 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="5" width="22" style="4" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -582,154 +605,164 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: Added event_status endpoint in excel
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G531QC\OneDrive\FSJS H8\Phase_3\final project\synapse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3844C8F9-EF9C-4A61-A54D-F295ACD9D4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F4A223-5CBD-4D2F-90EC-C56C40EBD952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9266" yWindow="-18514" windowWidth="17725" windowHeight="17880" xr2:uid="{D2D7A30A-FD97-4444-AF1F-0EF9A96489A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>SERVICE</t>
   </si>
@@ -164,6 +164,18 @@
     companyName: str
   }
 }</t>
+  </si>
+  <si>
+    <t>GET /events_status</t>
+  </si>
+  <si>
+    <t>[
+  {
+    EndpointId: INT (PK),
+    CompanyId: INT (FK),
+    status: STR
+  }
+]</t>
   </si>
 </sst>
 </file>
@@ -192,7 +204,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +223,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -224,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -246,6 +264,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,17 +605,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4C204F-1896-4A4F-BA1C-B4F55B5058F3}">
-  <dimension ref="A2:F15"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="22" style="4" customWidth="1"/>
     <col min="6" max="6" width="42.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
@@ -765,6 +789,18 @@
         <v>30</v>
       </c>
     </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:A4"/>

</xml_diff>

<commit_message>
Updated ERD and api docs
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G531QC\OneDrive\FSJS H8\Phase_3\final project\synapse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC25AE5A-2ECE-401C-9AC6-E059F607A699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BF79EB-875E-47E1-9F67-AACFD663AF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9266" yWindow="-18514" windowWidth="17725" windowHeight="17880" xr2:uid="{D2D7A30A-FD97-4444-AF1F-0EF9A96489A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>SERVICE</t>
   </si>
@@ -197,6 +197,13 @@
    companyName: str
    }
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> token: {
+    email: str,
+    CompanyId: INT,
+    companyName: str
+  }</t>
   </si>
 </sst>
 </file>
@@ -629,7 +636,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +698,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -700,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
docs: Updated excel api.xls
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G531QC\OneDrive\FSJS H8\Phase_3\final project\synapse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C16C4-D0BC-4DB7-BCA7-99E6A37C1CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BE854F-7D2C-4689-AA8A-48A286FF6A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{D2D7A30A-FD97-4444-AF1F-0EF9A96489A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D2D7A30A-FD97-4444-AF1F-0EF9A96489A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>miners</t>
   </si>
   <si>
-    <t>POST /getData</t>
-  </si>
-  <si>
     <t>body: endpoint, startDate, endDate</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>body: processName, caseId, eventName, name, department, time, CompanyId</t>
+  </si>
+  <si>
+    <t>POST /startminer</t>
   </si>
 </sst>
 </file>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4C204F-1896-4A4F-BA1C-B4F55B5058F3}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,10 +657,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -674,13 +674,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -689,13 +689,13 @@
     <row r="4" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -803,15 +803,15 @@
         <v>25</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -819,14 +819,14 @@
         <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:5" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -834,11 +834,11 @@
         <v>26</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>